<commit_message>
Solicitud gráfica rec310 mat 10 -tema3
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion01/SolicitudGrafica_MA_10_01_CO_REC310.xlsx
+++ b/fuentes/contenidos/grado10/guion01/SolicitudGrafica_MA_10_01_CO_REC310.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Desktop\Nueva carpeta (4)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado10\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -1784,15 +1784,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>452438</xdr:colOff>
+      <xdr:colOff>42863</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>255727</xdr:rowOff>
+      <xdr:rowOff>295275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>2243111</xdr:colOff>
+      <xdr:colOff>3271924</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>1206501</xdr:rowOff>
+      <xdr:rowOff>2009774</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1816,8 +1816,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16835438" y="10899915"/>
-          <a:ext cx="1790673" cy="950774"/>
+          <a:off x="16406813" y="12192000"/>
+          <a:ext cx="3229061" cy="1714499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1839,15 +1839,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>619124</xdr:colOff>
+      <xdr:colOff>154278</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>83955</xdr:rowOff>
+      <xdr:rowOff>17352</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>2039937</xdr:colOff>
+      <xdr:colOff>2128788</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1500185</xdr:rowOff>
+      <xdr:rowOff>1985493</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1863,8 +1863,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16994187" y="2203268"/>
-          <a:ext cx="1420813" cy="1416230"/>
+          <a:off x="16521179" y="2143708"/>
+          <a:ext cx="1974510" cy="1968141"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1913,15 +1913,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
+      <xdr:colOff>306543</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>500061</xdr:rowOff>
+      <xdr:rowOff>510592</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2794155</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>4476748</xdr:rowOff>
+      <xdr:rowOff>4324349</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1937,8 +1937,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16621124" y="5191124"/>
-          <a:ext cx="2595564" cy="3976687"/>
+          <a:off x="16670493" y="5644567"/>
+          <a:ext cx="2487612" cy="3813757"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1950,15 +1950,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>828675</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
+      <xdr:rowOff>295275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>61913</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2408328</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1238250</xdr:rowOff>
+      <xdr:rowOff>838200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1982,8 +1982,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16621125" y="10120313"/>
-          <a:ext cx="2919413" cy="1000125"/>
+          <a:off x="17192625" y="10629900"/>
+          <a:ext cx="1579653" cy="542925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2005,15 +2005,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>595312</xdr:colOff>
+      <xdr:colOff>115678</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>290026</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>154184</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2158092</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>2071687</xdr:rowOff>
+      <xdr:rowOff>1422797</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2029,8 +2029,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16978312" y="12882563"/>
-          <a:ext cx="3487935" cy="1928812"/>
+          <a:off x="16474866" y="13476198"/>
+          <a:ext cx="2042414" cy="1132771"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2757,8 +2757,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -2774,7 +2774,7 @@
     <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
     <col min="10" max="10" width="34.875" style="15" customWidth="1"/>
-    <col min="11" max="11" width="29.625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="43.625" style="15" customWidth="1"/>
     <col min="12" max="12" width="20.375" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" hidden="1" customWidth="1"/>
     <col min="14" max="15" width="10.875" style="2" hidden="1" customWidth="1"/>
@@ -3045,7 +3045,7 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
@@ -3209,7 +3209,7 @@
         <v>F4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
@@ -3250,7 +3250,7 @@
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="194.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>

</xml_diff>